<commit_message>
add a few more jobs, sort merged tasks
</commit_message>
<xml_diff>
--- a/tasks/task-merged.xlsx
+++ b/tasks/task-merged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bluba\Documents\school\2018-SP\CSCI7000\task-delegability\tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{509D8A78-432A-41C6-84A0-5834B0D5AFAD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53AC8635-A4A9-4367-A949-4FBB7EB03BF0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="273">
   <si>
     <t>Task description</t>
   </si>
@@ -66,9 +66,6 @@
     <t>choreographer</t>
   </si>
   <si>
-    <t>Design new clothing to manufacture and sell (similar to what a fashion designer might do)</t>
-  </si>
-  <si>
     <t>fashion designer</t>
   </si>
   <si>
@@ -90,18 +87,12 @@
     <t>Playing the guitar (or another musical instrument)</t>
   </si>
   <si>
-    <t>Scheduling an important business meeting with several coworkers</t>
-  </si>
-  <si>
     <t>business</t>
   </si>
   <si>
     <t>secretary</t>
   </si>
   <si>
-    <t>Scout and recruit college athletic players to professional teams based on assessment of player's performance (similar to what a talent scout does)</t>
-  </si>
-  <si>
     <t>hiring, assessment</t>
   </si>
   <si>
@@ -174,12 +165,6 @@
     <t>photographer</t>
   </si>
   <si>
-    <t>Recommend an outfit for you to wear</t>
-  </si>
-  <si>
-    <t>Picking out/choosing an outfit for you to wear</t>
-  </si>
-  <si>
     <t>Teaching you how to cook</t>
   </si>
   <si>
@@ -234,15 +219,9 @@
     <t>real estate agent</t>
   </si>
   <si>
-    <t>Recommend houses to buy that suit a potential home-buyer’s needs and budget (similar to part of what a real estate agent might do)</t>
-  </si>
-  <si>
     <t>real estate</t>
   </si>
   <si>
-    <t>Recommending products (e.g., clothing, kitchen items, electronics) for you to buy</t>
-  </si>
-  <si>
     <t>Assisting people in picking out and locating merchandise in a store, similar to what a retail sales assistant might do</t>
   </si>
   <si>
@@ -252,9 +231,6 @@
     <t>retail sales assistant</t>
   </si>
   <si>
-    <t>Translating an article from a foreign language to English</t>
-  </si>
-  <si>
     <t>translation</t>
   </si>
   <si>
@@ -264,9 +240,6 @@
     <t>translator</t>
   </si>
   <si>
-    <t>Translating an article you'd like to read into english from a foreign language</t>
-  </si>
-  <si>
     <t>Identifying safety hazards on a construction site (e.g. tripping hazards)</t>
   </si>
   <si>
@@ -444,9 +417,6 @@
     <t>home care</t>
   </si>
   <si>
-    <t>Buying a birthday present for an acquaintance</t>
-  </si>
-  <si>
     <t>shopping</t>
   </si>
   <si>
@@ -528,9 +498,6 @@
     <t>server</t>
   </si>
   <si>
-    <t>Choosing and ordering something for you to eat for dinner</t>
-  </si>
-  <si>
     <t>Picking what music to listen to at home</t>
   </si>
   <si>
@@ -564,9 +531,6 @@
     <t>Telling a joke</t>
   </si>
   <si>
-    <t>Picking up and driving a person wherever they need to go</t>
-  </si>
-  <si>
     <t>driving</t>
   </si>
   <si>
@@ -609,12 +573,6 @@
     <t>editor</t>
   </si>
   <si>
-    <t>Thinking of and choosing a topic to write a short story about</t>
-  </si>
-  <si>
-    <t>Writing a speech to give at your best friend's wedding</t>
-  </si>
-  <si>
     <t>Writing a short story or blog post (creative writing)</t>
   </si>
   <si>
@@ -627,9 +585,6 @@
     <t>media</t>
   </si>
   <si>
-    <t>Interview job applicants and rate candidates</t>
-  </si>
-  <si>
     <t>hiring</t>
   </si>
   <si>
@@ -639,12 +594,6 @@
     <t>Finding and removing inappropriate photos and videos from social media posts (content moderation)</t>
   </si>
   <si>
-    <t>Curb the spread of misinformation on social media by flagging misleading viral articles</t>
-  </si>
-  <si>
-    <t>Identify and flag online hate speech</t>
-  </si>
-  <si>
     <t>Picking which news stories to show to people on social media websites</t>
   </si>
   <si>
@@ -678,9 +627,6 @@
     <t>Writing reports and publishing updates on House/Senate/gubernatorial races during election day (election news coverage)</t>
   </si>
   <si>
-    <t>Recommending clothes for a clothing retail customer to try on/buy (retail sales assistant/stylist)</t>
-  </si>
-  <si>
     <t>visible recommendation</t>
   </si>
   <si>
@@ -690,21 +636,12 @@
     <t>Moving &amp; packing merchandise in a warehouse for shipping to customers</t>
   </si>
   <si>
-    <t>Analyzing and sorting legal documents, e.g. to find legal precedents for arguing a case in court</t>
-  </si>
-  <si>
     <t>In court, determining a defendant’s risk (e.g., in committing another crime or missing the court date), to help judges make decisions about bail, sentencing, or parole</t>
   </si>
   <si>
     <t>Playing chess</t>
   </si>
   <si>
-    <t>Identify people who attended a political rally</t>
-  </si>
-  <si>
-    <t>Predict the sexual orientation of a person</t>
-  </si>
-  <si>
     <t>Monitoring farm animals’ (e.g., cows) behavior, predicting health issues, and alerting the farmer.</t>
   </si>
   <si>
@@ -735,9 +672,6 @@
     <t>Teaching a religion's doctrine and practices to followers, similar to some of the responsibilities of clergy/religious leaders</t>
   </si>
   <si>
-    <t xml:space="preserve">Educate patients and their family/friends about various health conditions, similar to a small part of a Registered Nurse's responsibilities </t>
-  </si>
-  <si>
     <t>For patients with various health conditions, providing advice and emotional support to patients and their family members -- similar to a small part of what a Registered Nurse might do</t>
   </si>
   <si>
@@ -750,9 +684,6 @@
     <t>Designing buildings that meet the needs of the client, and ensure the design meets regulations and building codes, similar to part of what an architect might do</t>
   </si>
   <si>
-    <t>Coordinate and oversee construction of a building, e.g., consulting with engineers, surveyors, specialists, and construction workers -- similar to some of what an architect might do.</t>
-  </si>
-  <si>
     <t>Examining injured or ill patients and developing an individualized plan of care/rehabilitation that promotes movement and healing and reduces pain -- similar to some of what a physical therapist might do.</t>
   </si>
   <si>
@@ -777,9 +708,6 @@
     <t>Cutting, drying, and styling hair, similar to what a barber or hairstylist might do</t>
   </si>
   <si>
-    <t>Coordinate the movement of aircraft to maintain safe distances between them -- similar to what an air traffic controller might do</t>
-  </si>
-  <si>
     <t>Mental Health and Substance Abuse Social Workers</t>
   </si>
   <si>
@@ -820,6 +748,105 @@
   </si>
   <si>
     <t>Air Traffic Controller</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>Scouting and recruiting college athletic players to professional teams based on assessment of player's performance (similar to what a talent scout does)</t>
+  </si>
+  <si>
+    <t>Translating an article you'd like to read from a foreign language to English</t>
+  </si>
+  <si>
+    <t>Picking out and buying a birthday present for an acquaintance</t>
+  </si>
+  <si>
+    <t>decision ?</t>
+  </si>
+  <si>
+    <t>Choosing and ordering food for you to eat for dinner</t>
+  </si>
+  <si>
+    <t>Driving a passenger to their destination (similar to a taxi driver or chauffeur)</t>
+  </si>
+  <si>
+    <t>Picking a topic to write a short story about</t>
+  </si>
+  <si>
+    <t>Writing a speech/toast to give at your best friend's wedding</t>
+  </si>
+  <si>
+    <t>Recommending clothes for a clothing retail customer to try on/buy (similar to what a retail sales assistant/stylist might do)</t>
+  </si>
+  <si>
+    <t>Analyzing and sorting legal documents for important information, e.g. to find legal precedents for arguing a case in court (similar to some of what a paralegal might do)</t>
+  </si>
+  <si>
+    <t>monitoring</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>Software developer</t>
+  </si>
+  <si>
+    <t>Developing a cell phone/mobile application that meets customer requirements, similar to what a programmer/app developer might do</t>
+  </si>
+  <si>
+    <t>Bartender</t>
+  </si>
+  <si>
+    <t>Lifeguard</t>
+  </si>
+  <si>
+    <t>Deciding on an outfit for you to wear</t>
+  </si>
+  <si>
+    <t>Designing new clothing to manufacture and sell (similar to what a fashion designer might do)</t>
+  </si>
+  <si>
+    <t>Scheduling an important business meeting with several co-workers</t>
+  </si>
+  <si>
+    <t>Interviewing job applicants and rating candidates</t>
+  </si>
+  <si>
+    <t>Recommending a few outfits for you to wear</t>
+  </si>
+  <si>
+    <t>Recommending houses to buy that suit a potential home-buyer’s needs and budget (similar to part of what a real estate agent might do)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommending other products you might be interested in while you're shopping </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educating patients and their family/friends about various health conditions, similar to a small part of a Registered Nurse's responsibilities </t>
+  </si>
+  <si>
+    <t>Watching for and saving drowning people in a pool, similar to what a lifeguard would do</t>
+  </si>
+  <si>
+    <t>Coordinating and oversee construction of a building, e.g., consulting with engineers, surveyors, specialists, and construction workers -- similar to some of what an architect might do.</t>
+  </si>
+  <si>
+    <t>Coordinating the movement of aircraft to maintain safe distances between them -- similar to what an air traffic controller might do</t>
+  </si>
+  <si>
+    <t>Curbing the spread of misinformation on social media by flagging misleading viral articles</t>
+  </si>
+  <si>
+    <t>Identifying and flagging online hate speech</t>
+  </si>
+  <si>
+    <t>Identifying people who attended a political rally</t>
+  </si>
+  <si>
+    <t>Serving drinks to customers in a bar</t>
+  </si>
+  <si>
+    <t>Predicting the sexual orientation of a person</t>
   </si>
 </sst>
 </file>
@@ -1191,10 +1218,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1249,6 +1276,9 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
       <c r="F2">
         <v>3</v>
       </c>
@@ -1258,7 +1288,7 @@
     </row>
     <row r="3" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>258</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1269,16 +1299,19 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
       <c r="F3">
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -1289,16 +1322,19 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -1307,18 +1343,21 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -1327,7 +1366,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>240</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1335,258 +1377,300 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="H9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H8" t="s">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>112</v>
+      </c>
+      <c r="E12" t="s">
+        <v>240</v>
       </c>
       <c r="F12">
         <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>240</v>
       </c>
       <c r="F13">
         <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>39</v>
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>240</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" t="s">
-        <v>42</v>
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>240</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16">
-        <v>2.5</v>
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>240</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17">
-        <v>2.5</v>
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>77</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>240</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>240</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>2.5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>261</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -1594,36 +1678,36 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
       </c>
       <c r="F21">
-        <v>2.5</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>257</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -1631,56 +1715,62 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>240</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>2.5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>240</v>
       </c>
       <c r="F24">
         <v>3</v>
       </c>
-      <c r="G24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -1688,1083 +1778,1233 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
       </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
       <c r="F26">
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="H26" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>240</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" t="s">
+        <v>240</v>
+      </c>
+      <c r="F28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="B29" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="H29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>74</v>
+        <v>262</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
       </c>
       <c r="F30">
         <v>3</v>
-      </c>
-      <c r="G30" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>78</v>
+        <v>263</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
       </c>
       <c r="F31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
+      <c r="E32" t="s">
+        <v>240</v>
+      </c>
       <c r="F32">
         <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>242</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
       </c>
+      <c r="E33" t="s">
+        <v>240</v>
+      </c>
       <c r="F33">
         <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>77</v>
       </c>
       <c r="F34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
       </c>
+      <c r="E35" t="s">
+        <v>240</v>
+      </c>
       <c r="F35">
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>77</v>
       </c>
       <c r="F36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>240</v>
       </c>
       <c r="F37">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" t="s">
+        <v>184</v>
+      </c>
+      <c r="E38" t="s">
+        <v>240</v>
+      </c>
+      <c r="F38">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
         <v>10</v>
       </c>
+      <c r="E39" t="s">
+        <v>28</v>
+      </c>
       <c r="F39">
         <v>3</v>
-      </c>
-      <c r="G39" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
       </c>
       <c r="F40">
-        <v>3</v>
-      </c>
-      <c r="G40" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>191</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>184</v>
+      </c>
+      <c r="E41" t="s">
+        <v>77</v>
       </c>
       <c r="F41">
         <v>3</v>
-      </c>
-      <c r="G41" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>193</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>184</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
       </c>
       <c r="F42">
         <v>3</v>
       </c>
-      <c r="G42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="E43" t="s">
+        <v>28</v>
       </c>
       <c r="F43">
         <v>3</v>
-      </c>
-      <c r="G43" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>240</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" t="s">
+        <v>240</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" t="s">
+        <v>184</v>
+      </c>
+      <c r="E48" t="s">
+        <v>251</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>240</v>
+      </c>
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
+        <v>240</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" t="s">
+        <v>240</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" t="s">
+        <v>184</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="H53" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>240</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" t="s">
+        <v>184</v>
+      </c>
+      <c r="E55" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C57" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" t="s">
+        <v>112</v>
+      </c>
+      <c r="E57" t="s">
+        <v>240</v>
+      </c>
+      <c r="F57">
+        <v>3</v>
+      </c>
+      <c r="G57" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C58" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" t="s">
+        <v>112</v>
+      </c>
+      <c r="E58" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58">
+        <v>3</v>
+      </c>
+      <c r="G58" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" t="s">
+        <v>240</v>
+      </c>
+      <c r="F59">
+        <v>3</v>
+      </c>
+      <c r="G59" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C60" t="s">
+        <v>96</v>
+      </c>
+      <c r="D60" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" t="s">
+        <v>240</v>
+      </c>
+      <c r="F60">
+        <v>3</v>
+      </c>
+      <c r="G60" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C61" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" t="s">
+        <v>240</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C62" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" t="s">
+        <v>240</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C63" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" t="s">
+        <v>112</v>
+      </c>
+      <c r="E63" t="s">
+        <v>240</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="G63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44">
-        <v>3</v>
-      </c>
-      <c r="G44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45">
-        <v>3</v>
-      </c>
-      <c r="G45" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B65" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>77</v>
+      </c>
+      <c r="G65" t="s">
         <v>109</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C46" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" t="s">
-        <v>10</v>
-      </c>
-      <c r="F46">
-        <v>3</v>
-      </c>
-      <c r="G46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" s="2" t="s">
+    </row>
+    <row r="66" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" t="s">
         <v>112</v>
       </c>
-      <c r="C47" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47">
-        <v>3</v>
-      </c>
-      <c r="G47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" t="s">
-        <v>17</v>
-      </c>
-      <c r="F48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D49" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" t="s">
-        <v>118</v>
-      </c>
-      <c r="G50" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51">
-        <v>3</v>
-      </c>
-      <c r="G51" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C52" t="s">
-        <v>125</v>
-      </c>
-      <c r="G52" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C53" t="s">
-        <v>125</v>
-      </c>
-      <c r="D53" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53">
-        <v>2</v>
-      </c>
-      <c r="G53" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C54" t="s">
-        <v>131</v>
-      </c>
-      <c r="D54" t="s">
-        <v>17</v>
-      </c>
-      <c r="G54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" t="s">
-        <v>131</v>
-      </c>
-      <c r="D55" t="s">
-        <v>17</v>
-      </c>
-      <c r="G55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C56" t="s">
-        <v>131</v>
-      </c>
-      <c r="D56" t="s">
-        <v>17</v>
-      </c>
-      <c r="G56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C57" t="s">
-        <v>131</v>
-      </c>
-      <c r="D57" t="s">
-        <v>17</v>
-      </c>
-      <c r="F57">
-        <v>3</v>
-      </c>
-      <c r="G57" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" t="s">
-        <v>131</v>
-      </c>
-      <c r="D58" t="s">
-        <v>17</v>
-      </c>
-      <c r="F58">
-        <v>3</v>
-      </c>
-      <c r="G58" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C59" t="s">
-        <v>131</v>
-      </c>
-      <c r="F59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" t="s">
-        <v>131</v>
-      </c>
-      <c r="D60" t="s">
-        <v>17</v>
-      </c>
-      <c r="F60">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C61" t="s">
-        <v>131</v>
-      </c>
-      <c r="D61" t="s">
-        <v>17</v>
-      </c>
-      <c r="G61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" t="s">
-        <v>131</v>
-      </c>
-      <c r="D62" t="s">
-        <v>17</v>
-      </c>
-      <c r="F62">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C63" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" t="s">
-        <v>148</v>
-      </c>
-      <c r="D64" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64">
+      <c r="D66" t="s">
+        <v>112</v>
+      </c>
+      <c r="E66" t="s">
+        <v>240</v>
+      </c>
+      <c r="F66">
+        <v>3</v>
+      </c>
+      <c r="G66" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C67" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" t="s">
+        <v>184</v>
+      </c>
+      <c r="E67" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67">
         <v>2.5</v>
-      </c>
-      <c r="G64" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C65" t="s">
-        <v>151</v>
-      </c>
-      <c r="D65" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65">
-        <v>3</v>
-      </c>
-      <c r="G65" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C66" t="s">
-        <v>151</v>
-      </c>
-      <c r="D66" t="s">
-        <v>10</v>
-      </c>
-      <c r="F66">
-        <v>3</v>
-      </c>
-      <c r="G66" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67">
-        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>240</v>
+      </c>
+      <c r="F68">
+        <v>3</v>
+      </c>
+      <c r="G68" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>157</v>
+        <v>216</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>112</v>
+      </c>
+      <c r="E69" t="s">
+        <v>240</v>
       </c>
       <c r="F69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>72</v>
+        <v>217</v>
       </c>
       <c r="C70" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>112</v>
+      </c>
+      <c r="E70" t="s">
+        <v>240</v>
       </c>
       <c r="F70">
         <v>3</v>
       </c>
       <c r="G70" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>72</v>
+        <v>266</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>112</v>
+      </c>
+      <c r="E71" t="s">
+        <v>240</v>
       </c>
       <c r="F71">
         <v>3</v>
       </c>
       <c r="G71" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>72</v>
+        <v>219</v>
       </c>
       <c r="C72" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>240</v>
       </c>
       <c r="F72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G72" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>72</v>
+        <v>220</v>
       </c>
       <c r="C73" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>112</v>
+      </c>
+      <c r="E73" t="s">
+        <v>240</v>
       </c>
       <c r="F73">
         <v>3</v>
+      </c>
+      <c r="G73" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>72</v>
+        <v>224</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>112</v>
+      </c>
+      <c r="E74" t="s">
+        <v>240</v>
       </c>
       <c r="F74">
         <v>3</v>
       </c>
       <c r="G74" t="s">
-        <v>168</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>170</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>112</v>
+      </c>
+      <c r="E75" t="s">
+        <v>240</v>
       </c>
       <c r="F75">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G75" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>170</v>
+        <v>267</v>
       </c>
       <c r="C76" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>112</v>
+      </c>
+      <c r="E76" t="s">
+        <v>240</v>
       </c>
       <c r="F76">
         <v>3</v>
       </c>
-      <c r="H76" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>170</v>
+        <v>254</v>
       </c>
       <c r="C77" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>112</v>
+      </c>
+      <c r="E77" t="s">
+        <v>240</v>
       </c>
       <c r="F77">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>170</v>
+        <v>115</v>
       </c>
       <c r="C78" t="s">
-        <v>170</v>
-      </c>
-      <c r="D78" t="s">
-        <v>17</v>
-      </c>
-      <c r="F78">
-        <v>3</v>
+        <v>116</v>
+      </c>
+      <c r="E78" t="s">
+        <v>77</v>
+      </c>
+      <c r="G78" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>170</v>
+        <v>119</v>
       </c>
       <c r="C79" t="s">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="D79" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="E79" t="s">
+        <v>240</v>
       </c>
       <c r="F79">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="G79" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="C80" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D80" t="s">
-        <v>17</v>
+        <v>184</v>
+      </c>
+      <c r="E80" t="s">
+        <v>77</v>
       </c>
       <c r="F80">
         <v>3</v>
+      </c>
+      <c r="H80" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>179</v>
+        <v>28</v>
       </c>
       <c r="C81" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>184</v>
+      </c>
+      <c r="E81" t="s">
+        <v>77</v>
       </c>
       <c r="F81">
         <v>3</v>
-      </c>
-      <c r="G81" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B82" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C82" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>184</v>
+      </c>
+      <c r="E82" t="s">
+        <v>240</v>
       </c>
       <c r="F82">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>179</v>
+        <v>268</v>
       </c>
       <c r="C83" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>184</v>
+      </c>
+      <c r="E83" t="s">
+        <v>77</v>
       </c>
       <c r="F83">
         <v>3</v>
-      </c>
-      <c r="G83" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>120</v>
+        <v>269</v>
       </c>
       <c r="C84" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>184</v>
+      </c>
+      <c r="E84" t="s">
+        <v>77</v>
       </c>
       <c r="F84">
         <v>3</v>
@@ -2772,138 +3012,162 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>46</v>
+        <v>205</v>
       </c>
       <c r="C85" t="s">
-        <v>187</v>
+        <v>122</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
       <c r="E85" t="s">
-        <v>188</v>
-      </c>
-      <c r="G85" t="s">
-        <v>39</v>
+        <v>240</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>189</v>
+        <v>121</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="C86" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D86" t="s">
-        <v>17</v>
-      </c>
-      <c r="F86">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="E86" t="s">
+        <v>240</v>
+      </c>
+      <c r="G86" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>191</v>
+        <v>123</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
       <c r="C87" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E87" t="s">
+        <v>240</v>
       </c>
       <c r="G87" t="s">
-        <v>192</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>193</v>
+        <v>124</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>144</v>
+        <v>43</v>
       </c>
       <c r="C88" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D88" t="s">
-        <v>17</v>
-      </c>
-      <c r="F88">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="E88" t="s">
+        <v>240</v>
+      </c>
+      <c r="G88" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
       <c r="C89" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D89" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E89" t="s">
+        <v>240</v>
       </c>
       <c r="F89">
         <v>3</v>
+      </c>
+      <c r="G89" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>195</v>
+        <v>127</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
       <c r="C90" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D90" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E90" t="s">
+        <v>240</v>
       </c>
       <c r="F90">
         <v>3</v>
+      </c>
+      <c r="G90" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>196</v>
+        <v>243</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>197</v>
+        <v>129</v>
       </c>
       <c r="C91" t="s">
-        <v>151</v>
-      </c>
-      <c r="D91" t="s">
-        <v>198</v>
+        <v>122</v>
+      </c>
+      <c r="E91" t="s">
+        <v>240</v>
       </c>
       <c r="F91">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>199</v>
+        <v>130</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>200</v>
+        <v>46</v>
       </c>
       <c r="C92" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="D92" t="s">
-        <v>198</v>
+        <v>16</v>
+      </c>
+      <c r="E92" t="s">
+        <v>240</v>
       </c>
       <c r="F92">
         <v>3</v>
@@ -2911,146 +3175,185 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="C93" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="D93" t="s">
-        <v>198</v>
-      </c>
-      <c r="F93">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E93" t="s">
+        <v>240</v>
+      </c>
+      <c r="G93" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C94" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94" t="s">
+        <v>240</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C94" t="s">
-        <v>198</v>
-      </c>
-      <c r="D94" t="s">
-        <v>198</v>
-      </c>
-      <c r="F94">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>203</v>
+      <c r="B95" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="C95" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
       <c r="D95" t="s">
-        <v>198</v>
+        <v>184</v>
+      </c>
+      <c r="E95" t="s">
+        <v>28</v>
       </c>
       <c r="F95">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>204</v>
+        <v>135</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C96" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
       <c r="D96" t="s">
-        <v>198</v>
-      </c>
-      <c r="F96">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E96" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>31</v>
+        <v>213</v>
       </c>
       <c r="C97" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
       <c r="D97" t="s">
-        <v>198</v>
+        <v>112</v>
+      </c>
+      <c r="E97" t="s">
+        <v>240</v>
       </c>
       <c r="F97">
         <v>3</v>
       </c>
-      <c r="H97" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="C98" t="s">
-        <v>198</v>
+        <v>138</v>
       </c>
       <c r="D98" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E98" t="s">
+        <v>28</v>
       </c>
       <c r="F98">
-        <v>3</v>
+        <v>2.5</v>
+      </c>
+      <c r="G98" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="C99" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="D99" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E99" t="s">
+        <v>244</v>
       </c>
       <c r="F99">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>226</v>
+        <v>144</v>
       </c>
       <c r="C100" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D100" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E100" t="s">
+        <v>244</v>
       </c>
       <c r="F100">
         <v>3</v>
+      </c>
+      <c r="G100" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>31</v>
+        <v>183</v>
       </c>
       <c r="C101" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="D101" t="s">
-        <v>198</v>
+        <v>184</v>
+      </c>
+      <c r="E101" t="s">
+        <v>77</v>
       </c>
       <c r="F101">
         <v>3</v>
@@ -3058,70 +3361,79 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="C102" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="D102" t="s">
-        <v>198</v>
+        <v>184</v>
+      </c>
+      <c r="E102" t="s">
+        <v>240</v>
       </c>
       <c r="F102">
         <v>3</v>
-      </c>
-      <c r="H102" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>213</v>
+        <v>270</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="C103" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="D103" t="s">
-        <v>198</v>
+        <v>184</v>
+      </c>
+      <c r="E103" t="s">
+        <v>77</v>
       </c>
       <c r="F103">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>144</v>
+        <v>223</v>
       </c>
       <c r="C104" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D104" t="s">
-        <v>198</v>
+        <v>112</v>
+      </c>
+      <c r="E104" t="s">
+        <v>240</v>
       </c>
       <c r="F104">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>215</v>
+        <v>146</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C105" t="s">
-        <v>144</v>
+        <v>147</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D105" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E105" t="s">
+        <v>240</v>
       </c>
       <c r="F105">
         <v>3</v>
@@ -3129,425 +3441,637 @@
     </row>
     <row r="106" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>216</v>
+        <v>148</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>227</v>
+        <v>147</v>
+      </c>
+      <c r="C106" t="s">
+        <v>65</v>
       </c>
       <c r="D106" t="s">
-        <v>198</v>
-      </c>
-      <c r="F106">
-        <v>2.5</v>
-      </c>
-      <c r="H106" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E106" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>218</v>
+        <v>149</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="C107" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="D107" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E107" t="s">
+        <v>240</v>
       </c>
       <c r="F107">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="C108" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D108" t="s">
-        <v>198</v>
+        <v>184</v>
+      </c>
+      <c r="E108" t="s">
+        <v>240</v>
       </c>
       <c r="F108">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="C109" t="s">
-        <v>121</v>
+        <v>65</v>
       </c>
       <c r="D109" t="s">
-        <v>198</v>
+        <v>184</v>
+      </c>
+      <c r="E109" t="s">
+        <v>28</v>
       </c>
       <c r="F109">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>228</v>
+        <v>65</v>
       </c>
       <c r="C110" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="D110" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E110" t="s">
+        <v>240</v>
       </c>
       <c r="F110">
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+      <c r="G110" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>222</v>
+        <v>152</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C111" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D111" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E111" t="s">
+        <v>240</v>
       </c>
       <c r="F111">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G111" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>223</v>
+        <v>154</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>197</v>
+        <v>65</v>
       </c>
       <c r="C112" t="s">
-        <v>151</v>
+        <v>65</v>
       </c>
       <c r="D112" t="s">
-        <v>198</v>
+        <v>10</v>
+      </c>
+      <c r="E112" t="s">
+        <v>240</v>
       </c>
       <c r="F112">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="B113" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C113" t="s">
+        <v>65</v>
+      </c>
+      <c r="D113" t="s">
+        <v>16</v>
+      </c>
+      <c r="E113" t="s">
+        <v>240</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C114" t="s">
+        <v>65</v>
+      </c>
+      <c r="D114" t="s">
+        <v>16</v>
+      </c>
+      <c r="E114" t="s">
+        <v>77</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
+      </c>
+      <c r="G114" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C115" t="s">
+        <v>65</v>
+      </c>
+      <c r="D115" t="s">
+        <v>112</v>
+      </c>
+      <c r="E115" t="s">
+        <v>240</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C116" t="s">
+        <v>159</v>
+      </c>
+      <c r="D116" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" t="s">
+        <v>77</v>
+      </c>
+      <c r="F116">
+        <v>2</v>
+      </c>
+      <c r="G116" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C117" t="s">
+        <v>159</v>
+      </c>
+      <c r="D117" t="s">
+        <v>16</v>
+      </c>
+      <c r="E117" t="s">
+        <v>77</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+      <c r="H117" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C118" t="s">
+        <v>159</v>
+      </c>
+      <c r="D118" t="s">
+        <v>16</v>
+      </c>
+      <c r="E118" t="s">
+        <v>77</v>
+      </c>
+      <c r="F118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C119" t="s">
+        <v>159</v>
+      </c>
+      <c r="D119" t="s">
+        <v>16</v>
+      </c>
+      <c r="E119" t="s">
+        <v>77</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C120" t="s">
+        <v>159</v>
+      </c>
+      <c r="D120" t="s">
+        <v>16</v>
+      </c>
+      <c r="E120" t="s">
+        <v>240</v>
+      </c>
+      <c r="F120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C121" t="s">
+        <v>159</v>
+      </c>
+      <c r="D121" t="s">
+        <v>16</v>
+      </c>
+      <c r="E121" t="s">
+        <v>240</v>
+      </c>
+      <c r="F121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C122" t="s">
+        <v>159</v>
+      </c>
+      <c r="D122" t="s">
+        <v>184</v>
+      </c>
+      <c r="E122" t="s">
+        <v>77</v>
+      </c>
+      <c r="F122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C123" t="s">
+        <v>168</v>
+      </c>
+      <c r="D123" t="s">
+        <v>10</v>
+      </c>
+      <c r="E123" t="s">
+        <v>240</v>
+      </c>
+      <c r="F123">
+        <v>3</v>
+      </c>
+      <c r="G123" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C113" t="s">
-        <v>170</v>
-      </c>
-      <c r="D113" t="s">
-        <v>198</v>
-      </c>
-      <c r="F113">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C114" t="s">
-        <v>105</v>
-      </c>
-      <c r="D114" t="s">
-        <v>198</v>
-      </c>
-      <c r="F114">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D115" t="s">
-        <v>121</v>
-      </c>
-      <c r="F115">
-        <v>3</v>
-      </c>
-      <c r="G115" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D116" t="s">
-        <v>121</v>
-      </c>
-      <c r="F116">
-        <v>3</v>
-      </c>
-      <c r="G116" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D117" t="s">
-        <v>121</v>
-      </c>
-      <c r="F117">
-        <v>3</v>
-      </c>
-      <c r="G117" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D118" t="s">
-        <v>121</v>
-      </c>
-      <c r="F118">
-        <v>3</v>
-      </c>
-      <c r="G118" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D119" t="s">
-        <v>121</v>
-      </c>
-      <c r="F119">
-        <v>3</v>
-      </c>
-      <c r="G119" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D120" t="s">
-        <v>121</v>
-      </c>
-      <c r="F120">
-        <v>3</v>
-      </c>
-      <c r="G120" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D121" t="s">
-        <v>121</v>
-      </c>
-      <c r="F121">
-        <v>3</v>
-      </c>
-      <c r="G121" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D122" t="s">
-        <v>121</v>
-      </c>
-      <c r="F122">
-        <v>3</v>
-      </c>
-      <c r="G122" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D123" t="s">
-        <v>121</v>
-      </c>
-      <c r="F123">
-        <v>3</v>
-      </c>
-      <c r="G123" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>240</v>
+      <c r="B124" t="s">
+        <v>167</v>
+      </c>
+      <c r="C124" t="s">
+        <v>168</v>
       </c>
       <c r="D124" t="s">
-        <v>121</v>
+        <v>10</v>
+      </c>
+      <c r="E124" t="s">
+        <v>240</v>
       </c>
       <c r="F124">
         <v>3</v>
       </c>
-      <c r="G124" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>241</v>
+        <v>171</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C125" t="s">
+        <v>168</v>
       </c>
       <c r="D125" t="s">
-        <v>121</v>
+        <v>10</v>
+      </c>
+      <c r="E125" t="s">
+        <v>240</v>
       </c>
       <c r="F125">
         <v>3</v>
       </c>
       <c r="G125" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>242</v>
+        <v>173</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C126" t="s">
+        <v>168</v>
       </c>
       <c r="D126" t="s">
-        <v>121</v>
+        <v>10</v>
+      </c>
+      <c r="E126" t="s">
+        <v>240</v>
       </c>
       <c r="F126">
         <v>3</v>
       </c>
-      <c r="G126" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>243</v>
+        <v>174</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C127" t="s">
+        <v>175</v>
       </c>
       <c r="D127" t="s">
-        <v>121</v>
-      </c>
-      <c r="F127">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="E127" t="s">
+        <v>240</v>
       </c>
       <c r="G127" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>244</v>
+        <v>177</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C128" t="s">
+        <v>134</v>
       </c>
       <c r="D128" t="s">
-        <v>121</v>
+        <v>16</v>
+      </c>
+      <c r="E128" t="s">
+        <v>28</v>
       </c>
       <c r="F128">
         <v>3</v>
       </c>
-      <c r="G128" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>245</v>
+        <v>179</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C129" t="s">
+        <v>134</v>
       </c>
       <c r="D129" t="s">
-        <v>121</v>
-      </c>
-      <c r="F129">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="E129" t="s">
+        <v>28</v>
       </c>
       <c r="G129" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C130" t="s">
+        <v>134</v>
       </c>
       <c r="D130" t="s">
-        <v>121</v>
+        <v>16</v>
+      </c>
+      <c r="E130" t="s">
+        <v>77</v>
       </c>
       <c r="F130">
         <v>3</v>
-      </c>
-      <c r="G130" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C131" t="s">
+        <v>134</v>
       </c>
       <c r="D131" t="s">
-        <v>121</v>
+        <v>16</v>
+      </c>
+      <c r="E131" t="s">
+        <v>240</v>
       </c>
       <c r="F131">
         <v>3</v>
       </c>
-      <c r="G131" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>248</v>
+        <v>181</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C132" t="s">
+        <v>134</v>
       </c>
       <c r="D132" t="s">
-        <v>121</v>
+        <v>16</v>
+      </c>
+      <c r="E132" t="s">
+        <v>240</v>
       </c>
       <c r="F132">
         <v>3</v>
-      </c>
-      <c r="G132" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>249</v>
+        <v>197</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C133" t="s">
+        <v>134</v>
       </c>
       <c r="D133" t="s">
-        <v>121</v>
+        <v>184</v>
+      </c>
+      <c r="E133" t="s">
+        <v>240</v>
       </c>
       <c r="F133">
         <v>3</v>
       </c>
-      <c r="G133" t="s">
-        <v>263</v>
+    </row>
+    <row r="134" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C134" t="s">
+        <v>134</v>
+      </c>
+      <c r="D134" t="s">
+        <v>184</v>
+      </c>
+      <c r="E134" t="s">
+        <v>240</v>
+      </c>
+      <c r="F134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C135" t="s">
+        <v>134</v>
+      </c>
+      <c r="D135" t="s">
+        <v>112</v>
+      </c>
+      <c r="E135" t="s">
+        <v>240</v>
+      </c>
+      <c r="F135">
+        <v>3</v>
+      </c>
+      <c r="G135" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup scale="41" firstPageNumber="0" fitToHeight="2" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <sortState ref="A2:H136">
+    <sortCondition ref="C2:C136"/>
+    <sortCondition ref="B2:B136"/>
+  </sortState>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="62" firstPageNumber="0" fitToHeight="3" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>